<commit_message>
Added unit tests (Xunit) and tests using Cucumber.
</commit_message>
<xml_diff>
--- a/Test techniques assignment 1.xlsx
+++ b/Test techniques assignment 1.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hk/Documents/Undervisning/Test 2017/Assignments/Test techniques assignment 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\microsoftsucks\Documents\MEGA\2025_studie_softwareudvikler\semester1\software_quality_hk\uge11_ect_and_bvt\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0E6DFC-6A16-4BD0-AAA2-3372CB2DF426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Bus type</t>
   </si>
@@ -76,9 +88,6 @@
     <t>Mini (KFM)</t>
   </si>
   <si>
-    <t>Total price = IF * InitialFee + KF * (10*D1 + 8*D2 + 6*D3)</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -94,22 +103,40 @@
     <t>[100 -500]</t>
   </si>
   <si>
-    <t>Initial fee:</t>
-  </si>
-  <si>
     <t>Kilometer fee (kr/km):</t>
   </si>
   <si>
     <t>Distance (km):</t>
   </si>
   <si>
-    <t>[501 - 10000</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>[501 - 10000]</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Total price = IF * InitialFee + KF * (10 * D1 + 8 * D2 + 6 * D3)</t>
+  </si>
+  <si>
+    <t>Initial fee (IF):</t>
+  </si>
+  <si>
+    <t>"test"</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,6 +192,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -456,16 +486,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J6"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -495,75 +528,144 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>99</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <v>500</v>
+      </c>
+      <c r="G2" s="3">
+        <v>501</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="3">
+        <v>10001</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>99</v>
+      </c>
+      <c r="E4" s="3">
+        <v>99</v>
+      </c>
+      <c r="F4" s="3">
+        <v>99</v>
+      </c>
+      <c r="G4" s="3">
+        <v>99</v>
+      </c>
+      <c r="H4" s="3">
+        <v>99</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>401</v>
+      </c>
+      <c r="G5" s="3">
+        <v>401</v>
+      </c>
+      <c r="H5" s="3">
+        <v>401</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9500</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -577,96 +679,119 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="C8" s="3">
+        <v>2500</v>
+      </c>
+      <c r="D8" s="3">
+        <f>F18+D4*H13</f>
+        <v>3490</v>
+      </c>
+      <c r="E8" s="3">
+        <f>F18*C18+(E4*H13+E5*H14)*C22</f>
+        <v>4747</v>
+      </c>
+      <c r="F8" s="3">
+        <f>F18*C18+(F4*H13+F5*H14)*C22</f>
+        <v>9547</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F18*C19+(G4*H13+G5*H14+G6*H15)*C23</f>
+        <v>4522.3999999999996</v>
+      </c>
+      <c r="H8" s="3">
+        <f>F18*C19+(H4*H13+H5*H14+H6*H15)*C23</f>
+        <v>38718.799999999996</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -677,7 +802,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -685,12 +810,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -698,7 +823,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -706,9 +831,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -718,24 +843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>